<commit_message>
atualizando site com o material da aula 2
</commit_message>
<xml_diff>
--- a/referencias_extras.xlsx
+++ b/referencias_extras.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/curso-r/202102-r4ds-1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9366AA-4EEE-7A4F-8934-52A4DCAA90A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="24320" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>aula</t>
   </si>
@@ -33,7 +42,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -65,7 +74,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -79,7 +88,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -93,7 +102,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -107,7 +116,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -124,7 +133,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -144,7 +153,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -158,7 +167,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -175,7 +184,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -192,7 +201,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -206,7 +215,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -220,7 +229,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -234,7 +243,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -248,7 +257,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -262,7 +271,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -279,7 +288,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -293,7 +302,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -307,7 +316,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -321,7 +330,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -335,7 +344,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -352,7 +361,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -366,7 +375,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -383,7 +392,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -400,7 +409,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -417,7 +426,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -431,43 +440,45 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>https://curso-r.github.io/zen-do-r/index.html</t>
     </r>
+  </si>
+  <si>
+    <t>Pentaho</t>
+  </si>
+  <si>
+    <t>R on Pentaho Data Integration (PDI)</t>
+  </si>
+  <si>
+    <t>https://support.pentaho.com/hc/article_attachments/360005005891/Integrating%20R%20with%20PDI.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -503,26 +514,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,24 +531,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -674,7 +735,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -683,7 +744,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -692,7 +753,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -766,7 +827,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -774,7 +835,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -793,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,7 +884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1066,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1092,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1044,9 +1105,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1061,7 +1128,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1069,7 +1136,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1088,7 +1155,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1181,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1207,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +1233,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1259,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1218,7 +1285,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,7 +1311,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1337,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1363,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1389,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1335,9 +1402,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1351,7 +1424,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1370,7 +1443,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1473,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1499,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1525,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1551,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,7 +1577,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1530,7 +1603,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1556,7 +1629,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1582,7 +1655,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1608,7 +1681,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1621,521 +1694,538 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.9062" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.0312" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6719" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.85156" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="1" customWidth="1"/>
+    <col min="4" max="4" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s" s="2">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s" s="2">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s" s="2">
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s" s="2">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s" s="2">
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>2</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s" s="2">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s" s="2">
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s" s="2">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s" s="2">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>2</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s" s="2">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s" s="2">
+      <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="4">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>35</v>
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>3</v>
       </c>
-      <c r="B15" t="s" s="2">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>37</v>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>39</v>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>41</v>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>4</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>43</v>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" ht="13.55" customHeight="1">
+    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>4</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s" s="2">
-        <v>45</v>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="D20" t="s" s="2">
-        <v>48</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" ht="13.55" customHeight="1">
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s" s="2">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s" s="2">
-        <v>52</v>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s" s="2">
-        <v>54</v>
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
+    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>6</v>
       </c>
-      <c r="B24" t="s" s="2">
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s" s="2">
-        <v>56</v>
+      <c r="C24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
+    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="D25" t="s" s="2">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
+    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="D26" t="s" s="2">
-        <v>61</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" ht="13.55" customHeight="1">
+    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>7</v>
       </c>
-      <c r="B27" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="D27" t="s" s="2">
-        <v>64</v>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
+    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>4</v>
-      </c>
-      <c r="B28" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="D28" t="s" s="2">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" ht="13.55" customHeight="1">
+    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s" s="2">
-        <v>70</v>
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" ht="13.55" customHeight="1">
+    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>8</v>
       </c>
-      <c r="B30" t="s" s="2">
+      <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C30" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="D30" t="s" s="2">
-        <v>72</v>
+      <c r="C30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" ht="13.55" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" ht="13.55" customHeight="1">
+    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2143,7 +2233,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" ht="13.55" customHeight="1">
+    <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2152,36 +2242,39 @@
       <c r="F33" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="https://livro.curso-r.com/1-instalacao.html"/>
-    <hyperlink ref="D5" r:id="rId2" location="" tooltip="" display="https://rstudio.com/wp-content/uploads/2016/05/base-r.pdf"/>
-    <hyperlink ref="D6" r:id="rId3" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/rstudio-IDE-cheatsheet-portuguese.pdf"/>
-    <hyperlink ref="D7" r:id="rId4" location="" tooltip="" display="https://livro.curso-r.com/3-r-base.html"/>
-    <hyperlink ref="D8" r:id="rId5" location="" tooltip="" display="https://livro.curso-r.com/4-pacotes.html"/>
-    <hyperlink ref="D9" r:id="rId6" location="" tooltip="" display="https://livro.curso-r.com/5-importacao.html"/>
-    <hyperlink ref="D11" r:id="rId7" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/rproj-dir.html"/>
-    <hyperlink ref="D12" r:id="rId8" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/data-import.pdf"/>
-    <hyperlink ref="D13" r:id="rId9" location="" tooltip="" display="https://livro.curso-r.com/6-pipe.html"/>
-    <hyperlink ref="D14" r:id="rId10" location="" tooltip="" display="https://livro.curso-r.com/7-manipulacao.html"/>
-    <hyperlink ref="D15" r:id="rId11" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/data-wrangling-cheatsheet-portuguese.pdf"/>
-    <hyperlink ref="D16" r:id="rId12" location="" tooltip="" display="https://youtu.be/xnUo25VRH70"/>
-    <hyperlink ref="D17" r:id="rId13" location="" tooltip="" display="https://github.com/gadenbuie/tidyexplain"/>
-    <hyperlink ref="D18" r:id="rId14" location="" tooltip="" display="https://github.com/abjur/abjutils"/>
-    <hyperlink ref="D19" r:id="rId15" location="" tooltip="" display="https://dbplyr.tidyverse.org/articles/translation-verb.html"/>
-    <hyperlink ref="D20" r:id="rId16" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/ggplot2-cheatsheet-portuguese.pdf"/>
-    <hyperlink ref="D21" r:id="rId17" location="" tooltip="" display="https://livro.curso-r.com/8-graficos.html"/>
-    <hyperlink ref="D22" r:id="rId18" location="" tooltip="" display="https://ggrepel.slowkow.com/"/>
-    <hyperlink ref="D23" r:id="rId19" location="" tooltip="" display="https://plotly.com/ggplot2/"/>
-    <hyperlink ref="D24" r:id="rId20" location="" tooltip="" display="https://blog.curso-r.com/posts/2020-02-20-gghighlight/"/>
-    <hyperlink ref="D25" r:id="rId21" location="" tooltip="" display="https://www.curso-r.com/blog/2020-12-03-dicas-relatorios-r4ds1_tabelas/"/>
-    <hyperlink ref="D26" r:id="rId22" location="" tooltip="" display="https://www.curso-r.com/blog/2020-17-02-dicas-relatorios-r4ds1_graficos/"/>
-    <hyperlink ref="D27" r:id="rId23" location="" tooltip="" display="https://livro.curso-r.com/9-relatorios.html"/>
-    <hyperlink ref="D28" r:id="rId24" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/factors.pdf"/>
-    <hyperlink ref="D29" r:id="rId25" location="" tooltip="" display="https://style.tidyverse.org/"/>
-    <hyperlink ref="D30" r:id="rId26" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/index.html"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D20" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D25" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D21" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
adiciona links sobre comunidades
</commit_message>
<xml_diff>
--- a/referencias_extras.xlsx
+++ b/referencias_extras.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>aula</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Comunidades</t>
   </si>
   <si>
-    <t>R-Ladies</t>
+    <t>R-Ladies - Dashboard</t>
   </si>
   <si>
     <t>https://benubah.github.io/r-community-explorer/rladies.html</t>
@@ -344,6 +344,62 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>https://dplyr.tidyverse.org/reference/join.html</t>
+    </r>
+  </si>
+  <si>
+    <t>R Brasil - Grupo no telegram</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://t.me/rbrasiloficial</t>
+    </r>
+  </si>
+  <si>
+    <t>Apresentação sobre a R-Ladies São Paulo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://r-ladies-sao-paulo.github.io/RLadiesTheme/</t>
+    </r>
+  </si>
+  <si>
+    <t>Capítulos da R-Ladies no Brasil</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://github.com/R-Ladies-Sao-Paulo/RLadies-Brasil</t>
+    </r>
+  </si>
+  <si>
+    <t>Pacote dados - Base de dados traduzidas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://cienciadedatos.github.io/dados/</t>
     </r>
   </si>
   <si>
@@ -518,7 +574,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -543,6 +599,12 @@
       <u val="single"/>
       <sz val="11"/>
       <color indexed="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -985,17 +1047,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1023,10 +1085,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1274,12 +1336,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1566,7 +1628,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1594,10 +1656,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1848,7 +1910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2343,25 +2405,33 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
+      <c r="A31" s="4">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s" s="5">
+        <v>72</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s" s="5">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -2371,7 +2441,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>75</v>
@@ -2387,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>77</v>
@@ -2400,108 +2470,108 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s" s="5">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" ht="15" customHeight="1">
+    <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="D37" t="s" s="6">
-        <v>84</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" ht="15" customHeight="1">
+        <v>85</v>
+      </c>
+      <c r="D37" t="s" s="5">
+        <v>86</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="4">
         <v>6</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s" s="9">
-        <v>85</v>
-      </c>
-      <c r="D38" t="s" s="10">
-        <v>86</v>
-      </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s" s="5">
+        <v>88</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="C39" t="s" s="13">
-        <v>88</v>
-      </c>
-      <c r="D39" t="s" s="10">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
+      <c r="D39" t="s" s="5">
+        <v>90</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" ht="15" customHeight="1">
-      <c r="A40" s="14">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s" s="15">
-        <v>87</v>
-      </c>
-      <c r="C40" t="s" s="16">
-        <v>90</v>
-      </c>
-      <c r="D40" t="s" s="10">
+      <c r="A40" s="4">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" ht="13.55" customHeight="1">
-      <c r="A41" s="17">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s" s="16">
+      <c r="D40" t="s" s="6">
         <v>92</v>
       </c>
-      <c r="C41" t="s" s="16">
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" s="4">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s" s="9">
         <v>93</v>
       </c>
       <c r="D41" t="s" s="10">
@@ -2510,14 +2580,14 @@
       <c r="E41" s="11"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" ht="13.55" customHeight="1">
-      <c r="A42" s="17">
-        <v>8</v>
-      </c>
-      <c r="B42" t="s" s="16">
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" s="4">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="C42" t="s" s="16">
+      <c r="C42" t="s" s="13">
         <v>96</v>
       </c>
       <c r="D42" t="s" s="10">
@@ -2526,21 +2596,69 @@
       <c r="E42" s="11"/>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" ht="13.55" customHeight="1">
-      <c r="A43" s="18">
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" s="14">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s" s="15">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s" s="16">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s" s="10">
+        <v>99</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" s="17">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s" s="16">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s" s="16">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s" s="10">
+        <v>102</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" ht="13.55" customHeight="1">
+      <c r="A45" s="17">
         <v>8</v>
       </c>
-      <c r="B43" t="s" s="19">
-        <v>95</v>
-      </c>
-      <c r="C43" t="s" s="19">
-        <v>98</v>
-      </c>
-      <c r="D43" t="s" s="20">
-        <v>99</v>
-      </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="22"/>
+      <c r="B45" t="s" s="16">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s" s="16">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s" s="10">
+        <v>105</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" ht="13.55" customHeight="1">
+      <c r="A46" s="18">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s" s="19">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s" s="19">
+        <v>106</v>
+      </c>
+      <c r="D46" t="s" s="20">
+        <v>107</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2561,17 +2679,21 @@
     <hyperlink ref="D28" r:id="rId15" location="" tooltip="" display="https://dbplyr.tidyverse.org/articles/translation-verb.html"/>
     <hyperlink ref="D29" r:id="rId16" location="" tooltip="" display="https://www.garrickadenbuie.com/project/tidyexplain/"/>
     <hyperlink ref="D30" r:id="rId17" location="" tooltip="" display="https://dplyr.tidyverse.org/reference/join.html"/>
-    <hyperlink ref="D32" r:id="rId18" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/factors.pdf"/>
-    <hyperlink ref="D33" r:id="rId19" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/ggplot2-cheatsheet-portuguese.pdf"/>
-    <hyperlink ref="D34" r:id="rId20" location="" tooltip="" display="https://livro.curso-r.com/8-graficos.html"/>
-    <hyperlink ref="D35" r:id="rId21" location="" tooltip="" display="https://ggrepel.slowkow.com/"/>
-    <hyperlink ref="D36" r:id="rId22" location="" tooltip="" display="https://plotly.com/ggplot2/"/>
-    <hyperlink ref="D37" r:id="rId23" location="" tooltip="" display="https://blog.curso-r.com/posts/2020-02-20-gghighlight/"/>
-    <hyperlink ref="D39" r:id="rId24" location="" tooltip="" display="https://www.curso-r.com/blog/2020-12-03-dicas-relatorios-r4ds1_tabelas/"/>
-    <hyperlink ref="D40" r:id="rId25" location="" tooltip="" display="https://www.curso-r.com/blog/2020-17-02-dicas-relatorios-r4ds1_graficos/"/>
-    <hyperlink ref="D41" r:id="rId26" location="" tooltip="" display="https://livro.curso-r.com/9-relatorios.html"/>
-    <hyperlink ref="D42" r:id="rId27" location="" tooltip="" display="https://style.tidyverse.org/"/>
-    <hyperlink ref="D43" r:id="rId28" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/index.html"/>
+    <hyperlink ref="D31" r:id="rId18" location="" tooltip="" display="https://t.me/rbrasiloficial"/>
+    <hyperlink ref="D32" r:id="rId19" location="" tooltip="" display="https://r-ladies-sao-paulo.github.io/RLadiesTheme/"/>
+    <hyperlink ref="D33" r:id="rId20" location="" tooltip="" display="https://github.com/R-Ladies-Sao-Paulo/RLadies-Brasil"/>
+    <hyperlink ref="D34" r:id="rId21" location="" tooltip="" display="https://cienciadedatos.github.io/dados/"/>
+    <hyperlink ref="D35" r:id="rId22" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/factors.pdf"/>
+    <hyperlink ref="D36" r:id="rId23" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/ggplot2-cheatsheet-portuguese.pdf"/>
+    <hyperlink ref="D37" r:id="rId24" location="" tooltip="" display="https://livro.curso-r.com/8-graficos.html"/>
+    <hyperlink ref="D38" r:id="rId25" location="" tooltip="" display="https://ggrepel.slowkow.com/"/>
+    <hyperlink ref="D39" r:id="rId26" location="" tooltip="" display="https://plotly.com/ggplot2/"/>
+    <hyperlink ref="D40" r:id="rId27" location="" tooltip="" display="https://blog.curso-r.com/posts/2020-02-20-gghighlight/"/>
+    <hyperlink ref="D42" r:id="rId28" location="" tooltip="" display="https://www.curso-r.com/blog/2020-12-03-dicas-relatorios-r4ds1_tabelas/"/>
+    <hyperlink ref="D43" r:id="rId29" location="" tooltip="" display="https://www.curso-r.com/blog/2020-17-02-dicas-relatorios-r4ds1_graficos/"/>
+    <hyperlink ref="D44" r:id="rId30" location="" tooltip="" display="https://livro.curso-r.com/9-relatorios.html"/>
+    <hyperlink ref="D45" r:id="rId31" location="" tooltip="" display="https://style.tidyverse.org/"/>
+    <hyperlink ref="D46" r:id="rId32" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/index.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
duvidas de ggplot e referencias extras
</commit_message>
<xml_diff>
--- a/referencias_extras.xlsx
+++ b/referencias_extras.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>aula</t>
   </si>
@@ -389,6 +389,23 @@
     </r>
   </si>
   <si>
+    <t>Boas práticas</t>
+  </si>
+  <si>
+    <t>Capítulo do livro “Zen do R”:  .RData e .Rhistory</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://curso-r.github.io/zen-do-r/rdata-rhistory.html</t>
+    </r>
+  </si>
+  <si>
     <t>Pacote dados - Base de dados traduzidas</t>
   </si>
   <si>
@@ -445,6 +462,20 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>https://livro.curso-r.com/8-graficos.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Documentação da base sobre StarWars</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://dplyr.tidyverse.org/reference/starwars.html</t>
     </r>
   </si>
   <si>
@@ -758,7 +789,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -776,6 +807,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1910,7 +1944,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2457,23 +2491,23 @@
         <v>5</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s" s="2">
         <v>77</v>
       </c>
+      <c r="C34" t="s" s="6">
+        <v>78</v>
+      </c>
       <c r="D34" t="s" s="5">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>80</v>
@@ -2486,7 +2520,7 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s" s="2">
         <v>82</v>
@@ -2505,160 +2539,192 @@
         <v>5</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s" s="5">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s" s="5">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" ht="15" customHeight="1">
+    <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="4">
         <v>6</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="D40" t="s" s="6">
         <v>92</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" ht="15" customHeight="1">
+      <c r="D40" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="4">
         <v>6</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="C41" t="s" s="9">
-        <v>93</v>
-      </c>
-      <c r="D41" t="s" s="10">
+        <v>85</v>
+      </c>
+      <c r="C41" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
+      <c r="D41" t="s" s="5">
+        <v>95</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" s="4">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s" s="7">
+        <v>97</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" s="4">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s" s="10">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s" s="11">
+        <v>99</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" ht="15" customHeight="1">
+      <c r="A44" s="4">
         <v>7</v>
       </c>
-      <c r="B42" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="C42" t="s" s="13">
-        <v>96</v>
-      </c>
-      <c r="D42" t="s" s="10">
-        <v>97</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" s="14">
+      <c r="B44" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s" s="14">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s" s="11">
+        <v>102</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" s="4">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C45" t="s" s="14">
+        <v>103</v>
+      </c>
+      <c r="D45" t="s" s="11">
+        <v>104</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" ht="13.55" customHeight="1">
+      <c r="A46" s="15">
         <v>7</v>
       </c>
-      <c r="B43" t="s" s="15">
-        <v>95</v>
-      </c>
-      <c r="C43" t="s" s="16">
-        <v>98</v>
-      </c>
-      <c r="D43" t="s" s="10">
-        <v>99</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" ht="13.55" customHeight="1">
-      <c r="A44" s="17">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s" s="16">
-        <v>100</v>
-      </c>
-      <c r="C44" t="s" s="16">
-        <v>101</v>
-      </c>
-      <c r="D44" t="s" s="10">
-        <v>102</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" ht="13.55" customHeight="1">
-      <c r="A45" s="17">
+      <c r="B46" t="s" s="16">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s" s="17">
+        <v>106</v>
+      </c>
+      <c r="D46" t="s" s="11">
+        <v>107</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" ht="13.55" customHeight="1">
+      <c r="A47" s="18">
         <v>8</v>
       </c>
-      <c r="B45" t="s" s="16">
-        <v>103</v>
-      </c>
-      <c r="C45" t="s" s="16">
-        <v>104</v>
-      </c>
-      <c r="D45" t="s" s="10">
-        <v>105</v>
-      </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" ht="13.55" customHeight="1">
-      <c r="A46" s="18">
+      <c r="B47" t="s" s="17">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s" s="17">
+        <v>109</v>
+      </c>
+      <c r="D47" t="s" s="11">
+        <v>110</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" ht="13.55" customHeight="1">
+      <c r="A48" s="19">
         <v>8</v>
       </c>
-      <c r="B46" t="s" s="19">
-        <v>103</v>
-      </c>
-      <c r="C46" t="s" s="19">
-        <v>106</v>
-      </c>
-      <c r="D46" t="s" s="20">
-        <v>107</v>
-      </c>
-      <c r="E46" s="21"/>
-      <c r="F46" s="22"/>
+      <c r="B48" t="s" s="20">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s" s="20">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s" s="21">
+        <v>112</v>
+      </c>
+      <c r="E48" s="22"/>
+      <c r="F48" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2682,18 +2748,20 @@
     <hyperlink ref="D31" r:id="rId18" location="" tooltip="" display="https://t.me/rbrasiloficial"/>
     <hyperlink ref="D32" r:id="rId19" location="" tooltip="" display="https://r-ladies-sao-paulo.github.io/RLadiesTheme/"/>
     <hyperlink ref="D33" r:id="rId20" location="" tooltip="" display="https://github.com/R-Ladies-Sao-Paulo/RLadies-Brasil"/>
-    <hyperlink ref="D34" r:id="rId21" location="" tooltip="" display="https://cienciadedatos.github.io/dados/"/>
-    <hyperlink ref="D35" r:id="rId22" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/factors.pdf"/>
-    <hyperlink ref="D36" r:id="rId23" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/ggplot2-cheatsheet-portuguese.pdf"/>
-    <hyperlink ref="D37" r:id="rId24" location="" tooltip="" display="https://livro.curso-r.com/8-graficos.html"/>
-    <hyperlink ref="D38" r:id="rId25" location="" tooltip="" display="https://ggrepel.slowkow.com/"/>
-    <hyperlink ref="D39" r:id="rId26" location="" tooltip="" display="https://plotly.com/ggplot2/"/>
-    <hyperlink ref="D40" r:id="rId27" location="" tooltip="" display="https://blog.curso-r.com/posts/2020-02-20-gghighlight/"/>
-    <hyperlink ref="D42" r:id="rId28" location="" tooltip="" display="https://www.curso-r.com/blog/2020-12-03-dicas-relatorios-r4ds1_tabelas/"/>
-    <hyperlink ref="D43" r:id="rId29" location="" tooltip="" display="https://www.curso-r.com/blog/2020-17-02-dicas-relatorios-r4ds1_graficos/"/>
-    <hyperlink ref="D44" r:id="rId30" location="" tooltip="" display="https://livro.curso-r.com/9-relatorios.html"/>
-    <hyperlink ref="D45" r:id="rId31" location="" tooltip="" display="https://style.tidyverse.org/"/>
-    <hyperlink ref="D46" r:id="rId32" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/index.html"/>
+    <hyperlink ref="D34" r:id="rId21" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/rdata-rhistory.html"/>
+    <hyperlink ref="D35" r:id="rId22" location="" tooltip="" display="https://cienciadedatos.github.io/dados/"/>
+    <hyperlink ref="D36" r:id="rId23" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/factors.pdf"/>
+    <hyperlink ref="D37" r:id="rId24" location="" tooltip="" display="https://raw.githubusercontent.com/rstudio/cheatsheets/master/translations/portuguese/ggplot2-cheatsheet-portuguese.pdf"/>
+    <hyperlink ref="D38" r:id="rId25" location="" tooltip="" display="https://livro.curso-r.com/8-graficos.html"/>
+    <hyperlink ref="D39" r:id="rId26" location="" tooltip="" display="https://dplyr.tidyverse.org/reference/starwars.html"/>
+    <hyperlink ref="D40" r:id="rId27" location="" tooltip="" display="https://ggrepel.slowkow.com/"/>
+    <hyperlink ref="D41" r:id="rId28" location="" tooltip="" display="https://plotly.com/ggplot2/"/>
+    <hyperlink ref="D42" r:id="rId29" location="" tooltip="" display="https://blog.curso-r.com/posts/2020-02-20-gghighlight/"/>
+    <hyperlink ref="D44" r:id="rId30" location="" tooltip="" display="https://www.curso-r.com/blog/2020-12-03-dicas-relatorios-r4ds1_tabelas/"/>
+    <hyperlink ref="D45" r:id="rId31" location="" tooltip="" display="https://www.curso-r.com/blog/2020-17-02-dicas-relatorios-r4ds1_graficos/"/>
+    <hyperlink ref="D46" r:id="rId32" location="" tooltip="" display="https://livro.curso-r.com/9-relatorios.html"/>
+    <hyperlink ref="D47" r:id="rId33" location="" tooltip="" display="https://style.tidyverse.org/"/>
+    <hyperlink ref="D48" r:id="rId34" location="" tooltip="" display="https://curso-r.github.io/zen-do-r/index.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>